<commit_message>
artcats: added alternative title functionality; updated handling of ISBD punctuation
</commit_message>
<xml_diff>
--- a/output_files/styled_form.xlsx
+++ b/output_files/styled_form.xlsx
@@ -459,7 +459,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,7 +486,7 @@
     <row r="2" ht="10" customHeight="1">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>Date: 27 Oct 2025</t>
+          <t>Date: 08 Nov 2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="n"/>
@@ -659,6 +659,22 @@
         </is>
       </c>
       <c r="F10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="13" customHeight="1">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>*dummy*</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr"/>
+      <c r="C11" s="7" t="inlineStr"/>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr">
+        <is>
+          <t>Relocating to CSF</t>
+        </is>
+      </c>
+      <c r="F11" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>